<commit_message>
Finished City College Courses
</commit_message>
<xml_diff>
--- a/City College Courses.xlsx
+++ b/City College Courses.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
   <si>
     <t>Course Code</t>
   </si>
@@ -30,25 +30,275 @@
     <t>ANTH</t>
   </si>
   <si>
-    <t>Archaeology</t>
-  </si>
-  <si>
-    <t>Cross-Cultural Perspectives</t>
-  </si>
-  <si>
-    <t>Languages and Dialects in Cross-Cultural Perspective</t>
-  </si>
-  <si>
-    <t>Human Origins</t>
+    <t>ENGL</t>
+  </si>
+  <si>
+    <t>FIQWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIQWS </t>
+  </si>
+  <si>
+    <t>Freshman Composition</t>
+  </si>
+  <si>
+    <t>Composition for WCGI History and Culture</t>
+  </si>
+  <si>
+    <t>Composition for WCGI Literature</t>
+  </si>
+  <si>
+    <t>Composition for Individual and Society</t>
+  </si>
+  <si>
+    <t>Composition for Scientific World</t>
+  </si>
+  <si>
+    <t>Composition for Creative Expression</t>
+  </si>
+  <si>
+    <t>Composition for US Experience</t>
+  </si>
+  <si>
+    <t>Writing for the Humanities and the Arts</t>
+  </si>
+  <si>
+    <t>Writing for the Social Sciences</t>
+  </si>
+  <si>
+    <t>Writing for the Sciences</t>
+  </si>
+  <si>
+    <t>Writing for Engineers</t>
+  </si>
+  <si>
+    <t>FQUAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freshman Quantitative Analysis: Developing a Taste for Numbers </t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>Mathematics for the Contemporary World</t>
+  </si>
+  <si>
+    <t>Introduction to Probability and Statistics</t>
+  </si>
+  <si>
+    <t>BIO</t>
+  </si>
+  <si>
+    <t>CHEM</t>
+  </si>
+  <si>
+    <t>EAS</t>
+  </si>
+  <si>
+    <t>Biology: Human Biology</t>
+  </si>
+  <si>
+    <t>Exploring Chemistry: Energy and Environment</t>
+  </si>
+  <si>
+    <t>Perspectives on Global Warming</t>
+  </si>
+  <si>
+    <t>AES</t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
+    <t>MUS</t>
+  </si>
+  <si>
+    <t>THTR</t>
+  </si>
+  <si>
+    <t>Survey of World Architecture I</t>
+  </si>
+  <si>
+    <t>Introduction to Visual Arts of the World</t>
+  </si>
+  <si>
+    <t>Introduction to Music</t>
+  </si>
+  <si>
+    <t>Introduction to World Music</t>
+  </si>
+  <si>
+    <t>Introduction to Jazz</t>
+  </si>
+  <si>
+    <t>Introduction to Theatre</t>
+  </si>
+  <si>
+    <t>WHUM</t>
+  </si>
+  <si>
+    <t>Theatre History 1</t>
+  </si>
+  <si>
+    <t>Theatre History 2</t>
+  </si>
+  <si>
+    <t>Theatre History 3</t>
+  </si>
+  <si>
+    <t>World Humanities I</t>
+  </si>
+  <si>
+    <t>World Humanities II</t>
+  </si>
+  <si>
+    <t>World Humanities: Modern World Literature</t>
+  </si>
+  <si>
+    <t>ASIA</t>
+  </si>
+  <si>
+    <t>BLST</t>
+  </si>
+  <si>
+    <t>WCIV</t>
+  </si>
+  <si>
+    <t>HIST</t>
+  </si>
+  <si>
+    <t>General Anthropology</t>
+  </si>
+  <si>
+    <t>Asia and its Peoples</t>
+  </si>
+  <si>
+    <t>Contemporary Asia</t>
+  </si>
+  <si>
+    <t>Contemporary China</t>
+  </si>
+  <si>
+    <t>African Heritage: Caribbean-Brazilian Experience</t>
+  </si>
+  <si>
+    <t>World Civilizations I: Prehistory to 1500 AD</t>
+  </si>
+  <si>
+    <t>World Civilizations II:1500 AD to present</t>
+  </si>
+  <si>
+    <t>Early Modern Europe</t>
+  </si>
+  <si>
+    <t>Modern Europe</t>
+  </si>
+  <si>
+    <t>ECO</t>
+  </si>
+  <si>
+    <t>JWST</t>
+  </si>
+  <si>
+    <t>PSY</t>
+  </si>
+  <si>
+    <t>SOC</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>Principles of Microeconomics</t>
+  </si>
+  <si>
+    <t>Psychology of Religion</t>
+  </si>
+  <si>
+    <t>Psychology in Modern World</t>
+  </si>
+  <si>
+    <t>Individual, Group and Society: An Introduction to Sociology</t>
+  </si>
+  <si>
+    <t>Women’s/Gender Roles in Contemporary Society</t>
+  </si>
+  <si>
+    <t>ASTR</t>
+  </si>
+  <si>
+    <t>Methods in Astronomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAS </t>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>The Dynamic Earth</t>
+  </si>
+  <si>
+    <t>Introduction to Drug Abuse and Addiction</t>
+  </si>
+  <si>
+    <t>PSC</t>
+  </si>
+  <si>
+    <t>USSO</t>
+  </si>
+  <si>
+    <t>American Government and Politics</t>
+  </si>
+  <si>
+    <t>US Society</t>
+  </si>
+  <si>
+    <t>The United States: From Its Origins to 1877</t>
+  </si>
+  <si>
+    <t>The United States since 1865</t>
+  </si>
+  <si>
+    <t>PHIL</t>
+  </si>
+  <si>
+    <t>Intro to Philosophy</t>
+  </si>
+  <si>
+    <t>Logical Reasoning</t>
+  </si>
+  <si>
+    <t>History of Philosophy I: Ancient Philosophy</t>
+  </si>
+  <si>
+    <t>Ethics</t>
+  </si>
+  <si>
+    <t>Philosophy of Science</t>
+  </si>
+  <si>
+    <t>Bioethics</t>
+  </si>
+  <si>
+    <t>Political Ideas and Issues</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -75,8 +325,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,63 +642,647 @@
     <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>11000</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10103</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10105</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10108</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10111</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10113</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10115</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>21001</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>21002</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>21003</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>21007</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10050</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1">
+        <v>15000</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>17300</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10004</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1">
+        <v>11000</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1">
+        <v>10400</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1">
+        <v>23202</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1">
+        <v>10100</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10200</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="1">
+        <v>14500</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1">
+        <v>13100</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1">
+        <v>21100</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1">
+        <v>21200</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="1">
+        <v>21300</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1">
+        <v>10100</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="1">
+        <v>10200</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="1">
+        <v>10312</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>20000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+      <c r="B31" s="1">
+        <v>10100</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="1">
+        <v>10100</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="1">
+        <v>20200</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1">
+        <v>20500</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="1">
+        <v>10200</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="1">
+        <v>10100</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="1">
+        <v>10200</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1">
+        <v>20400</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="1">
+        <v>20600</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="1">
+        <v>10250</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="1">
+        <v>10411</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="1">
+        <v>10200</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="1">
+        <v>10500</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="1">
+        <v>30500</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="1">
+        <v>10100</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="1">
+        <v>10100</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>24100</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1">
+        <v>24100</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="1">
+        <v>10200</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="1">
         <v>20100</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>20200</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>20300</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+      <c r="C53" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="1">
+        <v>30500</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="1">
+        <v>30800</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="1">
+        <v>32200</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="1">
+        <v>34905</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="1">
+        <v>12400</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>